<commit_message>
Refactor functions to expression instead of statement
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6750" windowWidth="19200" windowHeight="6210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="19200" windowHeight="6210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beknopt" sheetId="2" r:id="rId1"/>
@@ -2501,31 +2501,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2540,31 +2531,40 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2578,11 +2578,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3014,11 +3014,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3043,14 +3043,14 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="90" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="104"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="91"/>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
@@ -3102,24 +3102,24 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="53"/>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="101" t="s">
         <v>163</v>
       </c>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="94"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="101"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="102"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="53"/>
       <c r="B12" s="39" t="s">
         <v>516</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="96"/>
+      <c r="D12" s="106"/>
       <c r="E12" s="35"/>
       <c r="F12" s="35" t="s">
         <v>15</v>
@@ -3141,10 +3141,10 @@
       <c r="B14" s="42" t="s">
         <v>517</v>
       </c>
-      <c r="C14" s="88" t="s">
+      <c r="C14" s="103" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="89"/>
+      <c r="D14" s="104"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="43"/>
@@ -3193,10 +3193,10 @@
       <c r="B19" s="42" t="s">
         <v>518</v>
       </c>
-      <c r="C19" s="90" t="s">
+      <c r="C19" s="92" t="s">
         <v>171</v>
       </c>
-      <c r="D19" s="91"/>
+      <c r="D19" s="93"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13" t="s">
         <v>18</v>
@@ -3207,10 +3207,10 @@
       <c r="B20" s="42" t="s">
         <v>519</v>
       </c>
-      <c r="C20" s="88" t="s">
+      <c r="C20" s="103" t="s">
         <v>165</v>
       </c>
-      <c r="D20" s="89"/>
+      <c r="D20" s="104"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13" t="s">
         <v>25</v>
@@ -3221,10 +3221,10 @@
       <c r="B21" s="42" t="s">
         <v>520</v>
       </c>
-      <c r="C21" s="90" t="s">
+      <c r="C21" s="92" t="s">
         <v>167</v>
       </c>
-      <c r="D21" s="91"/>
+      <c r="D21" s="93"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13" t="s">
         <v>29</v>
@@ -3235,10 +3235,10 @@
       <c r="B22" s="42" t="s">
         <v>521</v>
       </c>
-      <c r="C22" s="90" t="s">
+      <c r="C22" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="D22" s="91"/>
+      <c r="D22" s="93"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="8"/>
@@ -3247,10 +3247,10 @@
       <c r="B23" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="C23" s="90" t="s">
+      <c r="C23" s="92" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="91"/>
+      <c r="D23" s="93"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13" t="s">
         <v>39</v>
@@ -3261,10 +3261,10 @@
       <c r="B24" s="42" t="s">
         <v>523</v>
       </c>
-      <c r="C24" s="88" t="s">
+      <c r="C24" s="103" t="s">
         <v>168</v>
       </c>
-      <c r="D24" s="89"/>
+      <c r="D24" s="104"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13" t="s">
         <v>40</v>
@@ -3275,10 +3275,10 @@
       <c r="B25" s="42" t="s">
         <v>524</v>
       </c>
-      <c r="C25" s="88" t="s">
+      <c r="C25" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="D25" s="89"/>
+      <c r="D25" s="104"/>
       <c r="E25" s="36"/>
       <c r="F25" s="36"/>
       <c r="G25" s="37"/>
@@ -3297,10 +3297,10 @@
       <c r="B27" s="42" t="s">
         <v>525</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="103" t="s">
         <v>175</v>
       </c>
-      <c r="D27" s="89"/>
+      <c r="D27" s="104"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="2"/>
@@ -3319,10 +3319,10 @@
       <c r="B29" s="42" t="s">
         <v>526</v>
       </c>
-      <c r="C29" s="90" t="s">
+      <c r="C29" s="92" t="s">
         <v>202</v>
       </c>
-      <c r="D29" s="91"/>
+      <c r="D29" s="93"/>
       <c r="E29" s="40"/>
       <c r="F29" s="13"/>
       <c r="G29" s="2"/>
@@ -3341,10 +3341,10 @@
       <c r="B31" s="42" t="s">
         <v>527</v>
       </c>
-      <c r="C31" s="90" t="s">
+      <c r="C31" s="92" t="s">
         <v>201</v>
       </c>
-      <c r="D31" s="91"/>
+      <c r="D31" s="93"/>
       <c r="E31" s="40"/>
       <c r="F31" s="13"/>
       <c r="G31" s="2"/>
@@ -3353,10 +3353,10 @@
       <c r="B32" s="42" t="s">
         <v>528</v>
       </c>
-      <c r="C32" s="88" t="s">
+      <c r="C32" s="103" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="89"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="40"/>
       <c r="F32" s="13"/>
       <c r="G32" s="2"/>
@@ -3365,10 +3365,10 @@
       <c r="B33" s="42" t="s">
         <v>529</v>
       </c>
-      <c r="C33" s="90" t="s">
+      <c r="C33" s="92" t="s">
         <v>178</v>
       </c>
-      <c r="D33" s="91"/>
+      <c r="D33" s="93"/>
       <c r="E33" s="40"/>
       <c r="F33" s="13"/>
       <c r="G33" s="2"/>
@@ -3377,10 +3377,10 @@
       <c r="B34" s="42" t="s">
         <v>530</v>
       </c>
-      <c r="C34" s="88" t="s">
+      <c r="C34" s="103" t="s">
         <v>179</v>
       </c>
-      <c r="D34" s="89"/>
+      <c r="D34" s="104"/>
       <c r="E34" s="40"/>
       <c r="F34" s="13"/>
       <c r="G34" s="2"/>
@@ -3399,10 +3399,10 @@
       <c r="B36" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C36" s="90" t="s">
+      <c r="C36" s="92" t="s">
         <v>209</v>
       </c>
-      <c r="D36" s="91"/>
+      <c r="D36" s="93"/>
       <c r="E36" s="40"/>
       <c r="F36" s="13"/>
       <c r="G36" s="2"/>
@@ -3421,10 +3421,10 @@
       <c r="B38" s="42" t="s">
         <v>532</v>
       </c>
-      <c r="C38" s="90" t="s">
+      <c r="C38" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="D38" s="91"/>
+      <c r="D38" s="93"/>
       <c r="E38" s="40"/>
       <c r="F38" s="13"/>
       <c r="G38" s="2"/>
@@ -3445,10 +3445,10 @@
       <c r="B40" s="40" t="s">
         <v>533</v>
       </c>
-      <c r="C40" s="90" t="s">
+      <c r="C40" s="92" t="s">
         <v>186</v>
       </c>
-      <c r="D40" s="91"/>
+      <c r="D40" s="93"/>
       <c r="E40" s="40"/>
       <c r="F40" s="13"/>
       <c r="G40" s="2"/>
@@ -3458,10 +3458,10 @@
       <c r="B41" s="40" t="s">
         <v>534</v>
       </c>
-      <c r="C41" s="90" t="s">
+      <c r="C41" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="D41" s="91"/>
+      <c r="D41" s="93"/>
       <c r="E41" s="40"/>
       <c r="F41" s="13"/>
       <c r="G41" s="2"/>
@@ -3471,10 +3471,10 @@
       <c r="B42" s="40" t="s">
         <v>535</v>
       </c>
-      <c r="C42" s="90" t="s">
+      <c r="C42" s="92" t="s">
         <v>188</v>
       </c>
-      <c r="D42" s="91"/>
+      <c r="D42" s="93"/>
       <c r="E42" s="40"/>
       <c r="F42" s="13"/>
       <c r="G42" s="2"/>
@@ -3484,10 +3484,10 @@
       <c r="B43" s="40" t="s">
         <v>536</v>
       </c>
-      <c r="C43" s="90" t="s">
+      <c r="C43" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="D43" s="91"/>
+      <c r="D43" s="93"/>
       <c r="E43" s="30"/>
       <c r="F43" s="13"/>
       <c r="G43" s="2"/>
@@ -3508,10 +3508,10 @@
       <c r="B45" s="40" t="s">
         <v>537</v>
       </c>
-      <c r="C45" s="90" t="s">
+      <c r="C45" s="92" t="s">
         <v>204</v>
       </c>
-      <c r="D45" s="91"/>
+      <c r="D45" s="93"/>
       <c r="E45" s="27"/>
       <c r="F45" s="13"/>
       <c r="G45" s="2"/>
@@ -3521,10 +3521,10 @@
       <c r="B46" s="40" t="s">
         <v>538</v>
       </c>
-      <c r="C46" s="90" t="s">
+      <c r="C46" s="92" t="s">
         <v>199</v>
       </c>
-      <c r="D46" s="91"/>
+      <c r="D46" s="93"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
       <c r="G46" s="2"/>
@@ -3534,34 +3534,34 @@
       <c r="B47" s="40" t="s">
         <v>539</v>
       </c>
-      <c r="C47" s="99" t="s">
+      <c r="C47" s="96" t="s">
         <v>504</v>
       </c>
-      <c r="D47" s="100"/>
+      <c r="D47" s="97"/>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="53"/>
-      <c r="B48" s="97" t="s">
+      <c r="B48" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="97"/>
-      <c r="D48" s="97"/>
-      <c r="E48" s="97"/>
-      <c r="F48" s="97"/>
-      <c r="G48" s="98"/>
+      <c r="C48" s="94"/>
+      <c r="D48" s="94"/>
+      <c r="E48" s="94"/>
+      <c r="F48" s="94"/>
+      <c r="G48" s="95"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="53"/>
       <c r="B49" s="40" t="s">
         <v>540</v>
       </c>
-      <c r="C49" s="90" t="s">
+      <c r="C49" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="D49" s="91"/>
+      <c r="D49" s="93"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
       <c r="G49" s="2"/>
@@ -3577,24 +3577,24 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="53"/>
-      <c r="B51" s="97" t="s">
+      <c r="B51" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="97"/>
-      <c r="D51" s="97"/>
-      <c r="E51" s="97"/>
-      <c r="F51" s="97"/>
-      <c r="G51" s="98"/>
+      <c r="C51" s="94"/>
+      <c r="D51" s="94"/>
+      <c r="E51" s="94"/>
+      <c r="F51" s="94"/>
+      <c r="G51" s="95"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="53"/>
       <c r="B52" s="54" t="s">
         <v>541</v>
       </c>
-      <c r="C52" s="90" t="s">
+      <c r="C52" s="92" t="s">
         <v>189</v>
       </c>
-      <c r="D52" s="91"/>
+      <c r="D52" s="93"/>
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="2"/>
@@ -3615,10 +3615,10 @@
       <c r="B54" s="54" t="s">
         <v>542</v>
       </c>
-      <c r="C54" s="105" t="s">
+      <c r="C54" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="D54" s="106"/>
+      <c r="D54" s="99"/>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
       <c r="G54" s="2"/>
@@ -3639,10 +3639,10 @@
       <c r="B56" s="54" t="s">
         <v>543</v>
       </c>
-      <c r="C56" s="105" t="s">
+      <c r="C56" s="98" t="s">
         <v>190</v>
       </c>
-      <c r="D56" s="106"/>
+      <c r="D56" s="99"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="2"/>
@@ -3663,10 +3663,10 @@
       <c r="B58" s="54" t="s">
         <v>544</v>
       </c>
-      <c r="C58" s="90" t="s">
+      <c r="C58" s="92" t="s">
         <v>200</v>
       </c>
-      <c r="D58" s="91"/>
+      <c r="D58" s="93"/>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
       <c r="G58" s="2"/>
@@ -3676,10 +3676,10 @@
       <c r="B59" s="54" t="s">
         <v>545</v>
       </c>
-      <c r="C59" s="90" t="s">
+      <c r="C59" s="92" t="s">
         <v>206</v>
       </c>
-      <c r="D59" s="91"/>
+      <c r="D59" s="93"/>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="2"/>
@@ -3695,24 +3695,24 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="53"/>
-      <c r="B61" s="97" t="s">
+      <c r="B61" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="97"/>
-      <c r="D61" s="97"/>
-      <c r="E61" s="97"/>
-      <c r="F61" s="97"/>
-      <c r="G61" s="98"/>
+      <c r="C61" s="94"/>
+      <c r="D61" s="94"/>
+      <c r="E61" s="94"/>
+      <c r="F61" s="94"/>
+      <c r="G61" s="95"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="53"/>
       <c r="B62" s="54" t="s">
         <v>546</v>
       </c>
-      <c r="C62" s="99" t="s">
+      <c r="C62" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="D62" s="100"/>
+      <c r="D62" s="97"/>
       <c r="E62" s="13"/>
       <c r="F62" s="13"/>
       <c r="G62" s="2"/>
@@ -3722,10 +3722,10 @@
       <c r="B63" s="54" t="s">
         <v>547</v>
       </c>
-      <c r="C63" s="90" t="s">
+      <c r="C63" s="92" t="s">
         <v>196</v>
       </c>
-      <c r="D63" s="91"/>
+      <c r="D63" s="93"/>
       <c r="E63" s="13"/>
       <c r="F63" s="13"/>
       <c r="G63" s="2"/>
@@ -3735,10 +3735,10 @@
       <c r="B64" s="54" t="s">
         <v>548</v>
       </c>
-      <c r="C64" s="99" t="s">
+      <c r="C64" s="96" t="s">
         <v>197</v>
       </c>
-      <c r="D64" s="100"/>
+      <c r="D64" s="97"/>
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
       <c r="G64" s="2"/>
@@ -3748,18 +3748,18 @@
       <c r="B65" s="54" t="s">
         <v>549</v>
       </c>
-      <c r="C65" s="90" t="s">
+      <c r="C65" s="92" t="s">
         <v>205</v>
       </c>
-      <c r="D65" s="91"/>
+      <c r="D65" s="93"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="11"/>
-      <c r="C66" s="101"/>
-      <c r="D66" s="102"/>
+      <c r="C66" s="88"/>
+      <c r="D66" s="89"/>
       <c r="E66" s="15"/>
       <c r="F66" s="15"/>
       <c r="G66" s="3"/>
@@ -3774,6 +3774,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="C19:D19"/>
@@ -3790,31 +3815,6 @@
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="B48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C41:D41"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:G10 B49:G50 B52:G60 B62:G66 B12:G47">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -3830,8 +3830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J285"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="G99" sqref="G99"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="G160" sqref="G160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3844,11 +3844,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
       <c r="G1" s="75"/>
     </row>
     <row r="2" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="G3" s="85">
         <f>(J3/I3)</f>
-        <v>0.4</v>
+        <v>0.40583941605839419</v>
       </c>
       <c r="I3" s="86">
         <f>COUNT(G6:G11,G13:G62,G64:G130,G132:G270,G272:G283)*100</f>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="J3" s="87">
         <f>SUM(G6:G11,G13:G62,G64:G130,G132:G270,G272:G283)</f>
-        <v>10960</v>
+        <v>11120</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3892,10 +3892,10 @@
       <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="91"/>
+      <c r="D6" s="93"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
         <v>8</v>
@@ -3920,10 +3920,10 @@
       <c r="B8" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="C8" s="90" t="s">
+      <c r="C8" s="92" t="s">
         <v>505</v>
       </c>
-      <c r="D8" s="91"/>
+      <c r="D8" s="93"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="s">
         <v>8</v>
@@ -3936,10 +3936,10 @@
       <c r="B9" s="10" t="s">
         <v>510</v>
       </c>
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="92" t="s">
         <v>506</v>
       </c>
-      <c r="D9" s="91"/>
+      <c r="D9" s="93"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="s">
         <v>8</v>
@@ -3952,10 +3952,10 @@
       <c r="B10" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="92" t="s">
         <v>507</v>
       </c>
-      <c r="D10" s="91"/>
+      <c r="D10" s="93"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
         <v>8</v>
@@ -3968,10 +3968,10 @@
       <c r="B11" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="92" t="s">
         <v>508</v>
       </c>
-      <c r="D11" s="91"/>
+      <c r="D11" s="93"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13" t="s">
         <v>8</v>
@@ -3981,23 +3981,23 @@
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="98"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="95"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="89"/>
+      <c r="D13" s="104"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13" t="s">
         <v>9</v>
@@ -4010,10 +4010,10 @@
       <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="115" t="s">
+      <c r="C14" s="110" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="89"/>
+      <c r="D14" s="104"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13" t="s">
         <v>15</v>
@@ -4041,10 +4041,10 @@
       <c r="B16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="115" t="s">
+      <c r="C16" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="89"/>
+      <c r="D16" s="104"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="78">
@@ -4067,10 +4067,10 @@
       <c r="B18" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="89"/>
+      <c r="D18" s="104"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13" t="s">
         <v>18</v>
@@ -4093,10 +4093,10 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="90" t="s">
+      <c r="C20" s="92" t="s">
         <v>550</v>
       </c>
-      <c r="D20" s="91"/>
+      <c r="D20" s="93"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="79">
@@ -4119,10 +4119,10 @@
       <c r="B22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="115" t="s">
+      <c r="C22" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="89"/>
+      <c r="D22" s="104"/>
       <c r="E22" s="36"/>
       <c r="F22" s="36"/>
       <c r="G22" s="80">
@@ -4145,10 +4145,10 @@
       <c r="B24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="115" t="s">
+      <c r="C24" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="89"/>
+      <c r="D24" s="104"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="78">
@@ -4171,10 +4171,10 @@
       <c r="B26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="115" t="s">
+      <c r="C26" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="89"/>
+      <c r="D26" s="104"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13" t="s">
         <v>25</v>
@@ -4199,10 +4199,10 @@
       <c r="B28" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="115" t="s">
+      <c r="C28" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="89"/>
+      <c r="D28" s="104"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13" t="s">
         <v>29</v>
@@ -4230,10 +4230,10 @@
       <c r="B30" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="90" t="s">
+      <c r="C30" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="91"/>
+      <c r="D30" s="93"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13" t="s">
         <v>39</v>
@@ -4258,10 +4258,10 @@
       <c r="B32" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="90" t="s">
+      <c r="C32" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="91"/>
+      <c r="D32" s="93"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13" t="s">
         <v>40</v>
@@ -4314,10 +4314,10 @@
       <c r="B36" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="90" t="s">
+      <c r="C36" s="92" t="s">
         <v>211</v>
       </c>
-      <c r="D36" s="91"/>
+      <c r="D36" s="93"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="78">
@@ -4340,10 +4340,10 @@
       <c r="B38" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="90" t="s">
+      <c r="C38" s="92" t="s">
         <v>218</v>
       </c>
-      <c r="D38" s="91"/>
+      <c r="D38" s="93"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="78">
@@ -4366,10 +4366,10 @@
       <c r="B40" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="90" t="s">
+      <c r="C40" s="92" t="s">
         <v>224</v>
       </c>
-      <c r="D40" s="91"/>
+      <c r="D40" s="93"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="78">
@@ -4392,10 +4392,10 @@
       <c r="B42" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="90" t="s">
+      <c r="C42" s="92" t="s">
         <v>234</v>
       </c>
-      <c r="D42" s="91"/>
+      <c r="D42" s="93"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
       <c r="G42" s="78">
@@ -4418,10 +4418,10 @@
       <c r="B44" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C44" s="90" t="s">
+      <c r="C44" s="92" t="s">
         <v>238</v>
       </c>
-      <c r="D44" s="91"/>
+      <c r="D44" s="93"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="78">
@@ -4444,10 +4444,10 @@
       <c r="B46" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="90" t="s">
+      <c r="C46" s="92" t="s">
         <v>253</v>
       </c>
-      <c r="D46" s="91"/>
+      <c r="D46" s="93"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
       <c r="G46" s="78">
@@ -4470,10 +4470,10 @@
       <c r="B48" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="90" t="s">
+      <c r="C48" s="92" t="s">
         <v>268</v>
       </c>
-      <c r="D48" s="91"/>
+      <c r="D48" s="93"/>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
       <c r="G48" s="78">
@@ -4499,10 +4499,10 @@
       <c r="B50" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="90" t="s">
+      <c r="C50" s="92" t="s">
         <v>277</v>
       </c>
-      <c r="D50" s="91"/>
+      <c r="D50" s="93"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
       <c r="G50" s="78">
@@ -4525,10 +4525,10 @@
       <c r="B52" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C52" s="90" t="s">
+      <c r="C52" s="92" t="s">
         <v>284</v>
       </c>
-      <c r="D52" s="91"/>
+      <c r="D52" s="93"/>
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="78">
@@ -4557,10 +4557,10 @@
       <c r="B54" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C54" s="105" t="s">
+      <c r="C54" s="98" t="s">
         <v>290</v>
       </c>
-      <c r="D54" s="106"/>
+      <c r="D54" s="99"/>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
       <c r="G54" s="78">
@@ -4589,10 +4589,10 @@
       <c r="B56" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C56" s="90" t="s">
+      <c r="C56" s="92" t="s">
         <v>298</v>
       </c>
-      <c r="D56" s="91"/>
+      <c r="D56" s="93"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="78">
@@ -4621,10 +4621,10 @@
       <c r="B58" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="90" t="s">
+      <c r="C58" s="92" t="s">
         <v>309</v>
       </c>
-      <c r="D58" s="91"/>
+      <c r="D58" s="93"/>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
       <c r="G58" s="78">
@@ -4653,10 +4653,10 @@
       <c r="B60" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C60" s="105" t="s">
+      <c r="C60" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="106"/>
+      <c r="D60" s="99"/>
       <c r="E60" s="13"/>
       <c r="F60" s="13" t="s">
         <v>44</v>
@@ -4669,10 +4669,10 @@
       <c r="B61" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="105" t="s">
+      <c r="C61" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="D61" s="106"/>
+      <c r="D61" s="99"/>
       <c r="E61" s="13"/>
       <c r="F61" s="13" t="s">
         <v>44</v>
@@ -4685,10 +4685,10 @@
       <c r="B62" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="105" t="s">
+      <c r="C62" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="D62" s="106"/>
+      <c r="D62" s="99"/>
       <c r="E62" s="13"/>
       <c r="F62" s="13" t="s">
         <v>44</v>
@@ -4698,23 +4698,23 @@
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="116" t="s">
+      <c r="B63" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="97"/>
-      <c r="D63" s="97"/>
-      <c r="E63" s="97"/>
-      <c r="F63" s="97"/>
-      <c r="G63" s="98"/>
+      <c r="C63" s="94"/>
+      <c r="D63" s="94"/>
+      <c r="E63" s="94"/>
+      <c r="F63" s="94"/>
+      <c r="G63" s="95"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C64" s="90" t="s">
+      <c r="C64" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="D64" s="91"/>
+      <c r="D64" s="93"/>
       <c r="E64" s="13"/>
       <c r="F64" s="13" t="s">
         <v>15</v>
@@ -4727,10 +4727,10 @@
       <c r="B65" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C65" s="99" t="s">
+      <c r="C65" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="D65" s="100"/>
+      <c r="D65" s="97"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13" t="s">
         <v>73</v>
@@ -4755,10 +4755,10 @@
       <c r="B67" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C67" s="99" t="s">
+      <c r="C67" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="D67" s="100"/>
+      <c r="D67" s="97"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13" t="s">
         <v>15</v>
@@ -4798,10 +4798,10 @@
       <c r="B70" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C70" s="90" t="s">
+      <c r="C70" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="D70" s="91"/>
+      <c r="D70" s="93"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
       <c r="G70" s="78">
@@ -4824,10 +4824,10 @@
       <c r="B72" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C72" s="109" t="s">
+      <c r="C72" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="D72" s="110"/>
+      <c r="D72" s="116"/>
       <c r="E72" s="13"/>
       <c r="F72" s="13"/>
       <c r="G72" s="78">
@@ -4862,10 +4862,10 @@
       <c r="B75" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C75" s="90" t="s">
+      <c r="C75" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="D75" s="91"/>
+      <c r="D75" s="93"/>
       <c r="E75" s="13"/>
       <c r="F75" s="13" t="s">
         <v>18</v>
@@ -4890,10 +4890,10 @@
       <c r="B77" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C77" s="90" t="s">
+      <c r="C77" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="D77" s="91"/>
+      <c r="D77" s="93"/>
       <c r="E77" s="13"/>
       <c r="F77" s="13" t="s">
         <v>75</v>
@@ -4906,10 +4906,10 @@
       <c r="B78" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C78" s="90" t="s">
+      <c r="C78" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="D78" s="91"/>
+      <c r="D78" s="93"/>
       <c r="E78" s="13"/>
       <c r="F78" s="13" t="s">
         <v>25</v>
@@ -4934,10 +4934,10 @@
       <c r="B80" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C80" s="90" t="s">
+      <c r="C80" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="D80" s="91"/>
+      <c r="D80" s="93"/>
       <c r="E80" s="13"/>
       <c r="F80" s="13" t="s">
         <v>77</v>
@@ -4950,10 +4950,10 @@
       <c r="B81" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="90" t="s">
+      <c r="C81" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="D81" s="91"/>
+      <c r="D81" s="93"/>
       <c r="E81" s="13"/>
       <c r="F81" s="13" t="s">
         <v>29</v>
@@ -4978,10 +4978,10 @@
       <c r="B83" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C83" s="90" t="s">
+      <c r="C83" s="92" t="s">
         <v>78</v>
       </c>
-      <c r="D83" s="91"/>
+      <c r="D83" s="93"/>
       <c r="E83" s="13"/>
       <c r="F83" s="13" t="s">
         <v>79</v>
@@ -4994,10 +4994,10 @@
       <c r="B84" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C84" s="90" t="s">
+      <c r="C84" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D84" s="91"/>
+      <c r="D84" s="93"/>
       <c r="E84" s="13"/>
       <c r="F84" s="13" t="s">
         <v>40</v>
@@ -5022,10 +5022,10 @@
       <c r="B86" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C86" s="90" t="s">
+      <c r="C86" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="D86" s="91"/>
+      <c r="D86" s="93"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
       <c r="G86" s="78">
@@ -5036,10 +5036,10 @@
       <c r="B87" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C87" s="90" t="s">
+      <c r="C87" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="D87" s="91"/>
+      <c r="D87" s="93"/>
       <c r="E87" s="13"/>
       <c r="F87" s="13" t="s">
         <v>39</v>
@@ -5080,10 +5080,10 @@
       <c r="B90" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C90" s="90" t="s">
+      <c r="C90" s="92" t="s">
         <v>213</v>
       </c>
-      <c r="D90" s="91"/>
+      <c r="D90" s="93"/>
       <c r="E90" s="13"/>
       <c r="F90" s="13"/>
       <c r="G90" s="78">
@@ -5106,10 +5106,10 @@
       <c r="B92" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C92" s="90" t="s">
+      <c r="C92" s="92" t="s">
         <v>214</v>
       </c>
-      <c r="D92" s="91"/>
+      <c r="D92" s="93"/>
       <c r="E92" s="13"/>
       <c r="F92" s="13"/>
       <c r="G92" s="78">
@@ -5146,10 +5146,10 @@
       <c r="B95" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C95" s="90" t="s">
+      <c r="C95" s="92" t="s">
         <v>220</v>
       </c>
-      <c r="D95" s="91"/>
+      <c r="D95" s="93"/>
       <c r="E95" s="13"/>
       <c r="F95" s="13"/>
       <c r="G95" s="78">
@@ -5160,14 +5160,14 @@
       <c r="B96" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C96" s="90" t="s">
+      <c r="C96" s="92" t="s">
         <v>573</v>
       </c>
-      <c r="D96" s="91"/>
+      <c r="D96" s="93"/>
       <c r="E96" s="13"/>
       <c r="F96" s="13"/>
       <c r="G96" s="78">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
@@ -5179,31 +5179,31 @@
       <c r="E97" s="13"/>
       <c r="F97" s="13"/>
       <c r="G97" s="78">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C98" s="90" t="s">
+      <c r="C98" s="92" t="s">
         <v>575</v>
       </c>
-      <c r="D98" s="91"/>
+      <c r="D98" s="93"/>
       <c r="E98" s="13"/>
       <c r="F98" s="13"/>
       <c r="G98" s="78">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C99" s="90" t="s">
+      <c r="C99" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="D99" s="91"/>
+      <c r="D99" s="93"/>
       <c r="E99" s="13"/>
       <c r="F99" s="13"/>
       <c r="G99" s="78">
@@ -5226,10 +5226,10 @@
       <c r="B101" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C101" s="90" t="s">
+      <c r="C101" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="D101" s="91"/>
+      <c r="D101" s="93"/>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
       <c r="G101" s="78">
@@ -5240,10 +5240,10 @@
       <c r="B102" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C102" s="105" t="s">
+      <c r="C102" s="98" t="s">
         <v>236</v>
       </c>
-      <c r="D102" s="106"/>
+      <c r="D102" s="99"/>
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
       <c r="G102" s="78">
@@ -5266,10 +5266,10 @@
       <c r="B104" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C104" s="90" t="s">
+      <c r="C104" s="92" t="s">
         <v>237</v>
       </c>
-      <c r="D104" s="91"/>
+      <c r="D104" s="93"/>
       <c r="E104" s="13"/>
       <c r="F104" s="13"/>
       <c r="G104" s="78">
@@ -5280,10 +5280,10 @@
       <c r="B105" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C105" s="90" t="s">
+      <c r="C105" s="92" t="s">
         <v>240</v>
       </c>
-      <c r="D105" s="91"/>
+      <c r="D105" s="93"/>
       <c r="E105" s="13"/>
       <c r="F105" s="13"/>
       <c r="G105" s="78">
@@ -5306,10 +5306,10 @@
       <c r="B107" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C107" s="90" t="s">
+      <c r="C107" s="92" t="s">
         <v>241</v>
       </c>
-      <c r="D107" s="91"/>
+      <c r="D107" s="93"/>
       <c r="E107" s="13"/>
       <c r="F107" s="13"/>
       <c r="G107" s="78">
@@ -5323,10 +5323,10 @@
       <c r="B108" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C108" s="90" t="s">
+      <c r="C108" s="92" t="s">
         <v>255</v>
       </c>
-      <c r="D108" s="91"/>
+      <c r="D108" s="93"/>
       <c r="E108" s="13"/>
       <c r="F108" s="13"/>
       <c r="G108" s="78">
@@ -5589,10 +5589,10 @@
       <c r="B128" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="C128" s="105" t="s">
+      <c r="C128" s="98" t="s">
         <v>557</v>
       </c>
-      <c r="D128" s="106"/>
+      <c r="D128" s="99"/>
       <c r="E128" s="13"/>
       <c r="F128" s="13"/>
       <c r="G128" s="78">
@@ -5603,10 +5603,10 @@
       <c r="B129" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="C129" s="105" t="s">
+      <c r="C129" s="98" t="s">
         <v>558</v>
       </c>
-      <c r="D129" s="106"/>
+      <c r="D129" s="99"/>
       <c r="E129" s="13"/>
       <c r="F129" s="13"/>
       <c r="G129" s="78">
@@ -5617,10 +5617,10 @@
       <c r="B130" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="C130" s="105" t="s">
+      <c r="C130" s="98" t="s">
         <v>559</v>
       </c>
-      <c r="D130" s="106"/>
+      <c r="D130" s="99"/>
       <c r="E130" s="13"/>
       <c r="F130" s="13"/>
       <c r="G130" s="78">
@@ -5628,23 +5628,23 @@
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B131" s="116" t="s">
+      <c r="B131" s="109" t="s">
         <v>83</v>
       </c>
-      <c r="C131" s="97"/>
-      <c r="D131" s="97"/>
-      <c r="E131" s="97"/>
-      <c r="F131" s="97"/>
-      <c r="G131" s="98"/>
+      <c r="C131" s="94"/>
+      <c r="D131" s="94"/>
+      <c r="E131" s="94"/>
+      <c r="F131" s="94"/>
+      <c r="G131" s="95"/>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" s="10" t="s">
         <v>389</v>
       </c>
-      <c r="C132" s="90" t="s">
+      <c r="C132" s="92" t="s">
         <v>160</v>
       </c>
-      <c r="D132" s="91"/>
+      <c r="D132" s="93"/>
       <c r="E132" s="13"/>
       <c r="F132" s="13" t="s">
         <v>15</v>
@@ -5669,10 +5669,10 @@
       <c r="B134" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="C134" s="99" t="s">
+      <c r="C134" s="96" t="s">
         <v>560</v>
       </c>
-      <c r="D134" s="100"/>
+      <c r="D134" s="97"/>
       <c r="E134" s="13"/>
       <c r="F134" s="13" t="s">
         <v>15</v>
@@ -5697,10 +5697,10 @@
       <c r="B136" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="C136" s="90" t="s">
+      <c r="C136" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="D136" s="91"/>
+      <c r="D136" s="93"/>
       <c r="E136" s="13"/>
       <c r="F136" s="13"/>
       <c r="G136" s="78">
@@ -5726,10 +5726,10 @@
       <c r="B138" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="C138" s="90" t="s">
+      <c r="C138" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="D138" s="91"/>
+      <c r="D138" s="93"/>
       <c r="E138" s="13"/>
       <c r="F138" s="13"/>
       <c r="G138" s="78">
@@ -5752,10 +5752,10 @@
       <c r="B140" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="C140" s="90" t="s">
+      <c r="C140" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="D140" s="91"/>
+      <c r="D140" s="93"/>
       <c r="E140" s="13"/>
       <c r="F140" s="13" t="s">
         <v>18</v>
@@ -5771,10 +5771,10 @@
       <c r="B141" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="C141" s="90" t="s">
+      <c r="C141" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="D141" s="91"/>
+      <c r="D141" s="93"/>
       <c r="E141" s="13"/>
       <c r="F141" s="13" t="s">
         <v>25</v>
@@ -5790,10 +5790,10 @@
       <c r="B142" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="C142" s="90" t="s">
+      <c r="C142" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="D142" s="91"/>
+      <c r="D142" s="93"/>
       <c r="E142" s="13"/>
       <c r="F142" s="13" t="s">
         <v>29</v>
@@ -5818,10 +5818,10 @@
       <c r="B144" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="C144" s="99" t="s">
+      <c r="C144" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="D144" s="100"/>
+      <c r="D144" s="97"/>
       <c r="E144" s="13"/>
       <c r="F144" s="13"/>
       <c r="G144" s="78">
@@ -5832,10 +5832,10 @@
       <c r="B145" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="C145" s="90" t="s">
+      <c r="C145" s="92" t="s">
         <v>91</v>
       </c>
-      <c r="D145" s="91"/>
+      <c r="D145" s="93"/>
       <c r="E145" s="13"/>
       <c r="F145" s="13"/>
       <c r="G145" s="78">
@@ -5862,10 +5862,10 @@
       <c r="B147" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="C147" s="90" t="s">
+      <c r="C147" s="92" t="s">
         <v>94</v>
       </c>
-      <c r="D147" s="91"/>
+      <c r="D147" s="93"/>
       <c r="E147" s="13"/>
       <c r="F147" s="13" t="s">
         <v>39</v>
@@ -5878,26 +5878,26 @@
       <c r="B148" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="C148" s="90" t="s">
+      <c r="C148" s="92" t="s">
         <v>95</v>
       </c>
-      <c r="D148" s="91"/>
+      <c r="D148" s="93"/>
       <c r="E148" s="13"/>
       <c r="F148" s="13" t="s">
         <v>40</v>
       </c>
       <c r="G148" s="78">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="C149" s="90" t="s">
+      <c r="C149" s="92" t="s">
         <v>158</v>
       </c>
-      <c r="D149" s="91"/>
+      <c r="D149" s="93"/>
       <c r="E149" s="13"/>
       <c r="F149" s="13"/>
       <c r="G149" s="78">
@@ -5920,10 +5920,10 @@
       <c r="B151" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="C151" s="90" t="s">
+      <c r="C151" s="92" t="s">
         <v>215</v>
       </c>
-      <c r="D151" s="91"/>
+      <c r="D151" s="93"/>
       <c r="E151" s="13"/>
       <c r="F151" s="13"/>
       <c r="G151" s="78">
@@ -5934,10 +5934,10 @@
       <c r="B152" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="C152" s="99" t="s">
+      <c r="C152" s="96" t="s">
         <v>216</v>
       </c>
-      <c r="D152" s="100"/>
+      <c r="D152" s="97"/>
       <c r="E152" s="13"/>
       <c r="F152" s="13"/>
       <c r="G152" s="78">
@@ -5948,10 +5948,10 @@
       <c r="B153" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="C153" s="99" t="s">
+      <c r="C153" s="96" t="s">
         <v>221</v>
       </c>
-      <c r="D153" s="100"/>
+      <c r="D153" s="97"/>
       <c r="E153" s="13"/>
       <c r="F153" s="13"/>
       <c r="G153" s="78">
@@ -5962,10 +5962,10 @@
       <c r="B154" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="C154" s="99" t="s">
+      <c r="C154" s="96" t="s">
         <v>222</v>
       </c>
-      <c r="D154" s="100"/>
+      <c r="D154" s="97"/>
       <c r="E154" s="13"/>
       <c r="F154" s="13"/>
       <c r="G154" s="78">
@@ -5988,10 +5988,10 @@
       <c r="B156" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="C156" s="99" t="s">
+      <c r="C156" s="96" t="s">
         <v>226</v>
       </c>
-      <c r="D156" s="100"/>
+      <c r="D156" s="97"/>
       <c r="E156" s="13"/>
       <c r="F156" s="13"/>
       <c r="G156" s="78">
@@ -6002,10 +6002,10 @@
       <c r="B157" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="C157" s="99" t="s">
+      <c r="C157" s="96" t="s">
         <v>230</v>
       </c>
-      <c r="D157" s="100"/>
+      <c r="D157" s="97"/>
       <c r="E157" s="13"/>
       <c r="F157" s="13"/>
       <c r="G157" s="78">
@@ -6016,10 +6016,10 @@
       <c r="B158" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="C158" s="99" t="s">
+      <c r="C158" s="96" t="s">
         <v>231</v>
       </c>
-      <c r="D158" s="100"/>
+      <c r="D158" s="97"/>
       <c r="E158" s="13"/>
       <c r="F158" s="13"/>
       <c r="G158" s="78">
@@ -6042,10 +6042,10 @@
       <c r="B160" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="C160" s="99" t="s">
+      <c r="C160" s="96" t="s">
         <v>233</v>
       </c>
-      <c r="D160" s="100"/>
+      <c r="D160" s="97"/>
       <c r="E160" s="13"/>
       <c r="F160" s="13"/>
       <c r="G160" s="78">
@@ -6056,10 +6056,10 @@
       <c r="B161" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="C161" s="99" t="s">
+      <c r="C161" s="96" t="s">
         <v>242</v>
       </c>
-      <c r="D161" s="100"/>
+      <c r="D161" s="97"/>
       <c r="E161" s="13"/>
       <c r="F161" s="13"/>
       <c r="G161" s="78">
@@ -6070,10 +6070,10 @@
       <c r="B162" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="C162" s="99" t="s">
+      <c r="C162" s="96" t="s">
         <v>244</v>
       </c>
-      <c r="D162" s="100"/>
+      <c r="D162" s="97"/>
       <c r="E162" s="13"/>
       <c r="F162" s="13"/>
       <c r="G162" s="78">
@@ -6096,10 +6096,10 @@
       <c r="B164" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="C164" s="99" t="s">
+      <c r="C164" s="96" t="s">
         <v>245</v>
       </c>
-      <c r="D164" s="100"/>
+      <c r="D164" s="97"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
       <c r="G164" s="78">
@@ -6122,10 +6122,10 @@
       <c r="B166" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="C166" s="99" t="s">
+      <c r="C166" s="96" t="s">
         <v>324</v>
       </c>
-      <c r="D166" s="100"/>
+      <c r="D166" s="97"/>
       <c r="E166" s="13"/>
       <c r="F166" s="13"/>
       <c r="G166" s="78">
@@ -6136,10 +6136,10 @@
       <c r="B167" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="C167" s="99" t="s">
+      <c r="C167" s="96" t="s">
         <v>325</v>
       </c>
-      <c r="D167" s="100"/>
+      <c r="D167" s="97"/>
       <c r="E167" s="13"/>
       <c r="F167" s="13"/>
       <c r="G167" s="78">
@@ -6150,10 +6150,10 @@
       <c r="B168" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="C168" s="99" t="s">
+      <c r="C168" s="96" t="s">
         <v>326</v>
       </c>
-      <c r="D168" s="100"/>
+      <c r="D168" s="97"/>
       <c r="E168" s="13"/>
       <c r="F168" s="13"/>
       <c r="G168" s="78">
@@ -6164,10 +6164,10 @@
       <c r="B169" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="C169" s="99" t="s">
+      <c r="C169" s="96" t="s">
         <v>327</v>
       </c>
-      <c r="D169" s="100"/>
+      <c r="D169" s="97"/>
       <c r="E169" s="13"/>
       <c r="F169" s="13"/>
       <c r="G169" s="78">
@@ -6178,10 +6178,10 @@
       <c r="B170" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="C170" s="99" t="s">
+      <c r="C170" s="96" t="s">
         <v>328</v>
       </c>
-      <c r="D170" s="100"/>
+      <c r="D170" s="97"/>
       <c r="E170" s="13"/>
       <c r="F170" s="13"/>
       <c r="G170" s="78">
@@ -6192,10 +6192,10 @@
       <c r="B171" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="C171" s="99" t="s">
+      <c r="C171" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="D171" s="100"/>
+      <c r="D171" s="97"/>
       <c r="E171" s="13"/>
       <c r="F171" s="13"/>
       <c r="G171" s="78">
@@ -6206,10 +6206,10 @@
       <c r="B172" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="C172" s="99" t="s">
+      <c r="C172" s="96" t="s">
         <v>248</v>
       </c>
-      <c r="D172" s="100"/>
+      <c r="D172" s="97"/>
       <c r="E172" s="13"/>
       <c r="F172" s="13"/>
       <c r="G172" s="78">
@@ -6232,10 +6232,10 @@
       <c r="B174" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="C174" s="99" t="s">
+      <c r="C174" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="D174" s="100"/>
+      <c r="D174" s="97"/>
       <c r="E174" s="13"/>
       <c r="F174" s="13"/>
       <c r="G174" s="78">
@@ -6258,10 +6258,10 @@
       <c r="B176" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="C176" s="99" t="s">
+      <c r="C176" s="96" t="s">
         <v>252</v>
       </c>
-      <c r="D176" s="100"/>
+      <c r="D176" s="97"/>
       <c r="E176" s="13"/>
       <c r="F176" s="13"/>
       <c r="G176" s="78">
@@ -6275,10 +6275,10 @@
       <c r="B177" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="C177" s="99" t="s">
+      <c r="C177" s="96" t="s">
         <v>329</v>
       </c>
-      <c r="D177" s="100"/>
+      <c r="D177" s="97"/>
       <c r="E177" s="13"/>
       <c r="F177" s="13"/>
       <c r="G177" s="78">
@@ -6289,10 +6289,10 @@
       <c r="B178" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="C178" s="99" t="s">
+      <c r="C178" s="96" t="s">
         <v>330</v>
       </c>
-      <c r="D178" s="100"/>
+      <c r="D178" s="97"/>
       <c r="E178" s="13"/>
       <c r="F178" s="13"/>
       <c r="G178" s="78">
@@ -6303,10 +6303,10 @@
       <c r="B179" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="C179" s="99" t="s">
+      <c r="C179" s="96" t="s">
         <v>331</v>
       </c>
-      <c r="D179" s="100"/>
+      <c r="D179" s="97"/>
       <c r="E179" s="13"/>
       <c r="F179" s="13"/>
       <c r="G179" s="78">
@@ -6317,10 +6317,10 @@
       <c r="B180" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="C180" s="99" t="s">
+      <c r="C180" s="96" t="s">
         <v>332</v>
       </c>
-      <c r="D180" s="100"/>
+      <c r="D180" s="97"/>
       <c r="E180" s="13"/>
       <c r="F180" s="13"/>
       <c r="G180" s="78">
@@ -6331,10 +6331,10 @@
       <c r="B181" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="C181" s="99" t="s">
+      <c r="C181" s="96" t="s">
         <v>333</v>
       </c>
-      <c r="D181" s="100"/>
+      <c r="D181" s="97"/>
       <c r="E181" s="13"/>
       <c r="F181" s="13"/>
       <c r="G181" s="78">
@@ -6345,10 +6345,10 @@
       <c r="B182" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="C182" s="99" t="s">
+      <c r="C182" s="96" t="s">
         <v>259</v>
       </c>
-      <c r="D182" s="100"/>
+      <c r="D182" s="97"/>
       <c r="E182" s="13"/>
       <c r="F182" s="13"/>
       <c r="G182" s="78">
@@ -6411,10 +6411,10 @@
       <c r="B187" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="C187" s="99" t="s">
+      <c r="C187" s="96" t="s">
         <v>334</v>
       </c>
-      <c r="D187" s="100"/>
+      <c r="D187" s="97"/>
       <c r="E187" s="13"/>
       <c r="F187" s="13"/>
       <c r="G187" s="78">
@@ -6425,10 +6425,10 @@
       <c r="B188" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="C188" s="99" t="s">
+      <c r="C188" s="96" t="s">
         <v>335</v>
       </c>
-      <c r="D188" s="100"/>
+      <c r="D188" s="97"/>
       <c r="E188" s="13"/>
       <c r="F188" s="13"/>
       <c r="G188" s="78">
@@ -6439,10 +6439,10 @@
       <c r="B189" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="C189" s="99" t="s">
+      <c r="C189" s="96" t="s">
         <v>336</v>
       </c>
-      <c r="D189" s="100"/>
+      <c r="D189" s="97"/>
       <c r="E189" s="13"/>
       <c r="F189" s="13"/>
       <c r="G189" s="78">
@@ -6453,10 +6453,10 @@
       <c r="B190" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="C190" s="99" t="s">
+      <c r="C190" s="96" t="s">
         <v>337</v>
       </c>
-      <c r="D190" s="100"/>
+      <c r="D190" s="97"/>
       <c r="E190" s="13"/>
       <c r="F190" s="13"/>
       <c r="G190" s="78">
@@ -6467,10 +6467,10 @@
       <c r="B191" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="C191" s="99" t="s">
+      <c r="C191" s="96" t="s">
         <v>338</v>
       </c>
-      <c r="D191" s="100"/>
+      <c r="D191" s="97"/>
       <c r="E191" s="13"/>
       <c r="F191" s="13"/>
       <c r="G191" s="78">
@@ -6481,10 +6481,10 @@
       <c r="B192" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="C192" s="99" t="s">
+      <c r="C192" s="96" t="s">
         <v>371</v>
       </c>
-      <c r="D192" s="100"/>
+      <c r="D192" s="97"/>
       <c r="E192" s="13"/>
       <c r="F192" s="13"/>
       <c r="G192" s="78">
@@ -6561,10 +6561,10 @@
       <c r="B198" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="C198" s="99" t="s">
+      <c r="C198" s="96" t="s">
         <v>265</v>
       </c>
-      <c r="D198" s="100"/>
+      <c r="D198" s="97"/>
       <c r="E198" s="13"/>
       <c r="F198" s="13"/>
       <c r="G198" s="78">
@@ -6587,10 +6587,10 @@
       <c r="B200" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="C200" s="99" t="s">
+      <c r="C200" s="96" t="s">
         <v>339</v>
       </c>
-      <c r="D200" s="100"/>
+      <c r="D200" s="97"/>
       <c r="E200" s="13"/>
       <c r="F200" s="13"/>
       <c r="G200" s="78">
@@ -6613,10 +6613,10 @@
       <c r="B202" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="C202" s="99" t="s">
+      <c r="C202" s="96" t="s">
         <v>340</v>
       </c>
-      <c r="D202" s="100"/>
+      <c r="D202" s="97"/>
       <c r="E202" s="13"/>
       <c r="F202" s="13"/>
       <c r="G202" s="78">
@@ -6639,10 +6639,10 @@
       <c r="B204" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="C204" s="99" t="s">
+      <c r="C204" s="96" t="s">
         <v>341</v>
       </c>
-      <c r="D204" s="100"/>
+      <c r="D204" s="97"/>
       <c r="E204" s="13"/>
       <c r="F204" s="13"/>
       <c r="G204" s="78">
@@ -6665,10 +6665,10 @@
       <c r="B206" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="C206" s="99" t="s">
+      <c r="C206" s="96" t="s">
         <v>342</v>
       </c>
-      <c r="D206" s="100"/>
+      <c r="D206" s="97"/>
       <c r="E206" s="13"/>
       <c r="F206" s="13"/>
       <c r="G206" s="78">
@@ -6691,10 +6691,10 @@
       <c r="B208" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="C208" s="99" t="s">
+      <c r="C208" s="96" t="s">
         <v>343</v>
       </c>
-      <c r="D208" s="100"/>
+      <c r="D208" s="97"/>
       <c r="E208" s="13"/>
       <c r="F208" s="13"/>
       <c r="G208" s="78">
@@ -6717,10 +6717,10 @@
       <c r="B210" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="C210" s="99" t="s">
+      <c r="C210" s="96" t="s">
         <v>367</v>
       </c>
-      <c r="D210" s="100"/>
+      <c r="D210" s="97"/>
       <c r="E210" s="13"/>
       <c r="F210" s="13"/>
       <c r="G210" s="78">
@@ -6731,10 +6731,10 @@
       <c r="B211" s="10" t="s">
         <v>446</v>
       </c>
-      <c r="C211" s="99" t="s">
+      <c r="C211" s="96" t="s">
         <v>272</v>
       </c>
-      <c r="D211" s="100"/>
+      <c r="D211" s="97"/>
       <c r="E211" s="13"/>
       <c r="F211" s="13"/>
       <c r="G211" s="78">
@@ -6745,10 +6745,10 @@
       <c r="B212" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="C212" s="99" t="s">
+      <c r="C212" s="96" t="s">
         <v>273</v>
       </c>
-      <c r="D212" s="100"/>
+      <c r="D212" s="97"/>
       <c r="E212" s="13"/>
       <c r="F212" s="13"/>
       <c r="G212" s="78">
@@ -6771,10 +6771,10 @@
       <c r="B214" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="C214" s="99" t="s">
+      <c r="C214" s="96" t="s">
         <v>274</v>
       </c>
-      <c r="D214" s="100"/>
+      <c r="D214" s="97"/>
       <c r="E214" s="13"/>
       <c r="F214" s="13"/>
       <c r="G214" s="78">
@@ -6797,10 +6797,10 @@
       <c r="B216" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="C216" s="99" t="s">
+      <c r="C216" s="96" t="s">
         <v>275</v>
       </c>
-      <c r="D216" s="100"/>
+      <c r="D216" s="97"/>
       <c r="E216" s="13"/>
       <c r="F216" s="13"/>
       <c r="G216" s="78">
@@ -6811,10 +6811,10 @@
       <c r="B217" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="C217" s="99" t="s">
+      <c r="C217" s="96" t="s">
         <v>344</v>
       </c>
-      <c r="D217" s="100"/>
+      <c r="D217" s="97"/>
       <c r="E217" s="13"/>
       <c r="F217" s="13"/>
       <c r="G217" s="78">
@@ -6825,10 +6825,10 @@
       <c r="B218" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="C218" s="99" t="s">
+      <c r="C218" s="96" t="s">
         <v>345</v>
       </c>
-      <c r="D218" s="100"/>
+      <c r="D218" s="97"/>
       <c r="E218" s="13"/>
       <c r="F218" s="13"/>
       <c r="G218" s="78">
@@ -6839,10 +6839,10 @@
       <c r="B219" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="C219" s="99" t="s">
+      <c r="C219" s="96" t="s">
         <v>346</v>
       </c>
-      <c r="D219" s="100"/>
+      <c r="D219" s="97"/>
       <c r="E219" s="13"/>
       <c r="F219" s="13"/>
       <c r="G219" s="78">
@@ -6853,10 +6853,10 @@
       <c r="B220" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="C220" s="99" t="s">
+      <c r="C220" s="96" t="s">
         <v>347</v>
       </c>
-      <c r="D220" s="100"/>
+      <c r="D220" s="97"/>
       <c r="E220" s="13"/>
       <c r="F220" s="13"/>
       <c r="G220" s="78">
@@ -6867,10 +6867,10 @@
       <c r="B221" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="C221" s="99" t="s">
+      <c r="C221" s="96" t="s">
         <v>368</v>
       </c>
-      <c r="D221" s="100"/>
+      <c r="D221" s="97"/>
       <c r="E221" s="13"/>
       <c r="F221" s="13"/>
       <c r="G221" s="78">
@@ -6881,10 +6881,10 @@
       <c r="B222" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="C222" s="99" t="s">
+      <c r="C222" s="96" t="s">
         <v>281</v>
       </c>
-      <c r="D222" s="100"/>
+      <c r="D222" s="97"/>
       <c r="E222" s="13"/>
       <c r="F222" s="13"/>
       <c r="G222" s="78">
@@ -6895,10 +6895,10 @@
       <c r="B223" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="C223" s="99" t="s">
+      <c r="C223" s="96" t="s">
         <v>282</v>
       </c>
-      <c r="D223" s="100"/>
+      <c r="D223" s="97"/>
       <c r="E223" s="13"/>
       <c r="F223" s="13"/>
       <c r="G223" s="78">
@@ -6921,10 +6921,10 @@
       <c r="B225" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="C225" s="99" t="s">
+      <c r="C225" s="96" t="s">
         <v>283</v>
       </c>
-      <c r="D225" s="100"/>
+      <c r="D225" s="97"/>
       <c r="E225" s="13"/>
       <c r="F225" s="13"/>
       <c r="G225" s="78">
@@ -6947,10 +6947,10 @@
       <c r="B227" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="C227" s="99" t="s">
+      <c r="C227" s="96" t="s">
         <v>348</v>
       </c>
-      <c r="D227" s="100"/>
+      <c r="D227" s="97"/>
       <c r="E227" s="13"/>
       <c r="F227" s="13"/>
       <c r="G227" s="78">
@@ -6961,10 +6961,10 @@
       <c r="B228" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="C228" s="99" t="s">
+      <c r="C228" s="96" t="s">
         <v>349</v>
       </c>
-      <c r="D228" s="100"/>
+      <c r="D228" s="97"/>
       <c r="E228" s="13"/>
       <c r="F228" s="13"/>
       <c r="G228" s="78">
@@ -6975,10 +6975,10 @@
       <c r="B229" s="10" t="s">
         <v>460</v>
       </c>
-      <c r="C229" s="99" t="s">
+      <c r="C229" s="96" t="s">
         <v>350</v>
       </c>
-      <c r="D229" s="100"/>
+      <c r="D229" s="97"/>
       <c r="E229" s="13"/>
       <c r="F229" s="13"/>
       <c r="G229" s="78">
@@ -6989,10 +6989,10 @@
       <c r="B230" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="C230" s="99" t="s">
+      <c r="C230" s="96" t="s">
         <v>351</v>
       </c>
-      <c r="D230" s="100"/>
+      <c r="D230" s="97"/>
       <c r="E230" s="13"/>
       <c r="F230" s="13"/>
       <c r="G230" s="78">
@@ -7003,10 +7003,10 @@
       <c r="B231" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C231" s="99" t="s">
+      <c r="C231" s="96" t="s">
         <v>369</v>
       </c>
-      <c r="D231" s="100"/>
+      <c r="D231" s="97"/>
       <c r="E231" s="13"/>
       <c r="F231" s="13"/>
       <c r="G231" s="78">
@@ -7017,10 +7017,10 @@
       <c r="B232" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="C232" s="99" t="s">
+      <c r="C232" s="96" t="s">
         <v>288</v>
       </c>
-      <c r="D232" s="100"/>
+      <c r="D232" s="97"/>
       <c r="E232" s="13"/>
       <c r="F232" s="13"/>
       <c r="G232" s="78">
@@ -7031,10 +7031,10 @@
       <c r="B233" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="C233" s="99" t="s">
+      <c r="C233" s="96" t="s">
         <v>289</v>
       </c>
-      <c r="D233" s="100"/>
+      <c r="D233" s="97"/>
       <c r="E233" s="13"/>
       <c r="F233" s="13"/>
       <c r="G233" s="78">
@@ -7057,10 +7057,10 @@
       <c r="B235" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C235" s="99" t="s">
+      <c r="C235" s="96" t="s">
         <v>358</v>
       </c>
-      <c r="D235" s="100"/>
+      <c r="D235" s="97"/>
       <c r="E235" s="13"/>
       <c r="F235" s="13"/>
       <c r="G235" s="78">
@@ -7071,10 +7071,10 @@
       <c r="B236" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="C236" s="99" t="s">
+      <c r="C236" s="96" t="s">
         <v>359</v>
       </c>
-      <c r="D236" s="100"/>
+      <c r="D236" s="97"/>
       <c r="E236" s="13"/>
       <c r="F236" s="13"/>
       <c r="G236" s="78">
@@ -7085,10 +7085,10 @@
       <c r="B237" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="C237" s="99" t="s">
+      <c r="C237" s="96" t="s">
         <v>360</v>
       </c>
-      <c r="D237" s="100"/>
+      <c r="D237" s="97"/>
       <c r="E237" s="13"/>
       <c r="F237" s="13"/>
       <c r="G237" s="78">
@@ -7099,10 +7099,10 @@
       <c r="B238" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="C238" s="99" t="s">
+      <c r="C238" s="96" t="s">
         <v>361</v>
       </c>
-      <c r="D238" s="100"/>
+      <c r="D238" s="97"/>
       <c r="E238" s="13"/>
       <c r="F238" s="13"/>
       <c r="G238" s="78">
@@ -7113,10 +7113,10 @@
       <c r="B239" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="C239" s="99" t="s">
+      <c r="C239" s="96" t="s">
         <v>370</v>
       </c>
-      <c r="D239" s="100"/>
+      <c r="D239" s="97"/>
       <c r="E239" s="13"/>
       <c r="F239" s="13"/>
       <c r="G239" s="78">
@@ -7127,10 +7127,10 @@
       <c r="B240" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="C240" s="99" t="s">
+      <c r="C240" s="96" t="s">
         <v>294</v>
       </c>
-      <c r="D240" s="100"/>
+      <c r="D240" s="97"/>
       <c r="E240" s="13"/>
       <c r="F240" s="13"/>
       <c r="G240" s="78">
@@ -7141,10 +7141,10 @@
       <c r="B241" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="C241" s="99" t="s">
+      <c r="C241" s="96" t="s">
         <v>313</v>
       </c>
-      <c r="D241" s="100"/>
+      <c r="D241" s="97"/>
       <c r="E241" s="13"/>
       <c r="F241" s="13"/>
       <c r="G241" s="78">
@@ -7167,10 +7167,10 @@
       <c r="B243" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="C243" s="99" t="s">
+      <c r="C243" s="96" t="s">
         <v>362</v>
       </c>
-      <c r="D243" s="100"/>
+      <c r="D243" s="97"/>
       <c r="E243" s="13"/>
       <c r="F243" s="13"/>
       <c r="G243" s="78">
@@ -7181,10 +7181,10 @@
       <c r="B244" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="C244" s="99" t="s">
+      <c r="C244" s="96" t="s">
         <v>363</v>
       </c>
-      <c r="D244" s="100"/>
+      <c r="D244" s="97"/>
       <c r="E244" s="13"/>
       <c r="F244" s="13"/>
       <c r="G244" s="78">
@@ -7195,10 +7195,10 @@
       <c r="B245" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="C245" s="99" t="s">
+      <c r="C245" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="D245" s="100"/>
+      <c r="D245" s="97"/>
       <c r="E245" s="13"/>
       <c r="F245" s="13"/>
       <c r="G245" s="78">
@@ -7209,10 +7209,10 @@
       <c r="B246" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="C246" s="99" t="s">
+      <c r="C246" s="96" t="s">
         <v>365</v>
       </c>
-      <c r="D246" s="100"/>
+      <c r="D246" s="97"/>
       <c r="E246" s="13"/>
       <c r="F246" s="13"/>
       <c r="G246" s="78">
@@ -7223,10 +7223,10 @@
       <c r="B247" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="C247" s="99" t="s">
+      <c r="C247" s="96" t="s">
         <v>366</v>
       </c>
-      <c r="D247" s="100"/>
+      <c r="D247" s="97"/>
       <c r="E247" s="13"/>
       <c r="F247" s="13"/>
       <c r="G247" s="78">
@@ -7237,10 +7237,10 @@
       <c r="B248" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="C248" s="99" t="s">
+      <c r="C248" s="96" t="s">
         <v>303</v>
       </c>
-      <c r="D248" s="100"/>
+      <c r="D248" s="97"/>
       <c r="E248" s="13"/>
       <c r="F248" s="13"/>
       <c r="G248" s="78">
@@ -7263,10 +7263,10 @@
       <c r="B250" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="C250" s="99" t="s">
+      <c r="C250" s="96" t="s">
         <v>304</v>
       </c>
-      <c r="D250" s="100"/>
+      <c r="D250" s="97"/>
       <c r="E250" s="13"/>
       <c r="F250" s="13"/>
       <c r="G250" s="78">
@@ -7289,10 +7289,10 @@
       <c r="B252" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="C252" s="99" t="s">
+      <c r="C252" s="96" t="s">
         <v>306</v>
       </c>
-      <c r="D252" s="100"/>
+      <c r="D252" s="97"/>
       <c r="E252" s="13"/>
       <c r="F252" s="13"/>
       <c r="G252" s="78">
@@ -7315,10 +7315,10 @@
       <c r="B254" s="10" t="s">
         <v>480</v>
       </c>
-      <c r="C254" s="99" t="s">
+      <c r="C254" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="D254" s="100"/>
+      <c r="D254" s="97"/>
       <c r="E254" s="13"/>
       <c r="F254" s="13"/>
       <c r="G254" s="78">
@@ -7341,10 +7341,10 @@
       <c r="B256" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="C256" s="99" t="s">
+      <c r="C256" s="96" t="s">
         <v>314</v>
       </c>
-      <c r="D256" s="100"/>
+      <c r="D256" s="97"/>
       <c r="E256" s="13"/>
       <c r="F256" s="13"/>
       <c r="G256" s="78">
@@ -7355,10 +7355,10 @@
       <c r="B257" s="10" t="s">
         <v>482</v>
       </c>
-      <c r="C257" s="99" t="s">
+      <c r="C257" s="96" t="s">
         <v>315</v>
       </c>
-      <c r="D257" s="100"/>
+      <c r="D257" s="97"/>
       <c r="E257" s="13"/>
       <c r="F257" s="13"/>
       <c r="G257" s="78">
@@ -7381,10 +7381,10 @@
       <c r="B259" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C259" s="99" t="s">
+      <c r="C259" s="96" t="s">
         <v>317</v>
       </c>
-      <c r="D259" s="100"/>
+      <c r="D259" s="97"/>
       <c r="E259" s="13"/>
       <c r="F259" s="13"/>
       <c r="G259" s="78">
@@ -7407,10 +7407,10 @@
       <c r="B261" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="C261" s="99" t="s">
+      <c r="C261" s="96" t="s">
         <v>319</v>
       </c>
-      <c r="D261" s="100"/>
+      <c r="D261" s="97"/>
       <c r="E261" s="13"/>
       <c r="F261" s="13"/>
       <c r="G261" s="78">
@@ -7421,10 +7421,10 @@
       <c r="B262" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="C262" s="99" t="s">
+      <c r="C262" s="96" t="s">
         <v>322</v>
       </c>
-      <c r="D262" s="100"/>
+      <c r="D262" s="97"/>
       <c r="E262" s="13"/>
       <c r="F262" s="13"/>
       <c r="G262" s="78">
@@ -7435,10 +7435,10 @@
       <c r="B263" s="10" t="s">
         <v>486</v>
       </c>
-      <c r="C263" s="99" t="s">
+      <c r="C263" s="96" t="s">
         <v>320</v>
       </c>
-      <c r="D263" s="100"/>
+      <c r="D263" s="97"/>
       <c r="E263" s="13"/>
       <c r="F263" s="13"/>
       <c r="G263" s="78">
@@ -7449,10 +7449,10 @@
       <c r="B264" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="C264" s="99" t="s">
+      <c r="C264" s="96" t="s">
         <v>321</v>
       </c>
-      <c r="D264" s="100"/>
+      <c r="D264" s="97"/>
       <c r="E264" s="13"/>
       <c r="F264" s="13"/>
       <c r="G264" s="78">
@@ -7463,10 +7463,10 @@
       <c r="B265" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="C265" s="99" t="s">
+      <c r="C265" s="96" t="s">
         <v>323</v>
       </c>
-      <c r="D265" s="100"/>
+      <c r="D265" s="97"/>
       <c r="E265" s="13"/>
       <c r="F265" s="13"/>
       <c r="G265" s="78">
@@ -7477,10 +7477,10 @@
       <c r="B266" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="C266" s="99" t="s">
+      <c r="C266" s="96" t="s">
         <v>372</v>
       </c>
-      <c r="D266" s="100"/>
+      <c r="D266" s="97"/>
       <c r="E266" s="13"/>
       <c r="F266" s="13"/>
       <c r="G266" s="78">
@@ -7491,10 +7491,10 @@
       <c r="B267" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="C267" s="99" t="s">
+      <c r="C267" s="96" t="s">
         <v>374</v>
       </c>
-      <c r="D267" s="100"/>
+      <c r="D267" s="97"/>
       <c r="E267" s="13"/>
       <c r="F267" s="13"/>
       <c r="G267" s="78">
@@ -7505,10 +7505,10 @@
       <c r="B268" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="C268" s="105" t="s">
+      <c r="C268" s="98" t="s">
         <v>96</v>
       </c>
-      <c r="D268" s="106"/>
+      <c r="D268" s="99"/>
       <c r="E268" s="13"/>
       <c r="F268" s="13"/>
       <c r="G268" s="78">
@@ -7519,10 +7519,10 @@
       <c r="B269" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="C269" s="105" t="s">
+      <c r="C269" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="D269" s="106"/>
+      <c r="D269" s="99"/>
       <c r="E269" s="13"/>
       <c r="F269" s="13"/>
       <c r="G269" s="78">
@@ -7533,10 +7533,10 @@
       <c r="B270" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="C270" s="105" t="s">
+      <c r="C270" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="D270" s="106"/>
+      <c r="D270" s="99"/>
       <c r="E270" s="13"/>
       <c r="F270" s="13"/>
       <c r="G270" s="78">
@@ -7557,10 +7557,10 @@
       <c r="B272" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="C272" s="90" t="s">
+      <c r="C272" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="D272" s="91"/>
+      <c r="D272" s="93"/>
       <c r="E272" s="13"/>
       <c r="F272" s="13" t="s">
         <v>34</v>
@@ -7573,10 +7573,10 @@
       <c r="B273" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="C273" s="90" t="s">
+      <c r="C273" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="D273" s="91"/>
+      <c r="D273" s="93"/>
       <c r="E273" s="13"/>
       <c r="F273" s="13" t="s">
         <v>34</v>
@@ -7589,10 +7589,10 @@
       <c r="B274" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="C274" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D274" s="91"/>
+      <c r="C274" s="92" t="s">
+        <v>100</v>
+      </c>
+      <c r="D274" s="93"/>
       <c r="E274" s="13"/>
       <c r="F274" s="13"/>
       <c r="G274" s="78">
@@ -7615,10 +7615,10 @@
       <c r="B276" s="10" t="s">
         <v>497</v>
       </c>
-      <c r="C276" s="90" t="s">
+      <c r="C276" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="D276" s="91"/>
+      <c r="D276" s="93"/>
       <c r="E276" s="13"/>
       <c r="F276" s="13" t="s">
         <v>104</v>
@@ -7650,10 +7650,10 @@
       <c r="B278" s="10" t="s">
         <v>499</v>
       </c>
-      <c r="C278" s="90" t="s">
+      <c r="C278" s="92" t="s">
         <v>105</v>
       </c>
-      <c r="D278" s="91"/>
+      <c r="D278" s="93"/>
       <c r="E278" s="13"/>
       <c r="F278" s="13" t="s">
         <v>157</v>
@@ -7692,10 +7692,10 @@
       <c r="B281" s="34" t="s">
         <v>501</v>
       </c>
-      <c r="C281" s="105" t="s">
+      <c r="C281" s="98" t="s">
         <v>107</v>
       </c>
-      <c r="D281" s="106"/>
+      <c r="D281" s="99"/>
       <c r="E281" s="14"/>
       <c r="F281" s="14" t="s">
         <v>44</v>
@@ -7708,10 +7708,10 @@
       <c r="B282" s="34" t="s">
         <v>502</v>
       </c>
-      <c r="C282" s="105" t="s">
+      <c r="C282" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="D282" s="106"/>
+      <c r="D282" s="99"/>
       <c r="E282" s="14"/>
       <c r="F282" s="14" t="s">
         <v>44</v>
@@ -7724,10 +7724,10 @@
       <c r="B283" s="34" t="s">
         <v>503</v>
       </c>
-      <c r="C283" s="105" t="s">
+      <c r="C283" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="D283" s="106"/>
+      <c r="D283" s="99"/>
       <c r="E283" s="14"/>
       <c r="F283" s="14" t="s">
         <v>44</v>
@@ -7738,8 +7738,8 @@
     </row>
     <row r="284" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B284" s="11"/>
-      <c r="C284" s="101"/>
-      <c r="D284" s="102"/>
+      <c r="C284" s="88"/>
+      <c r="D284" s="89"/>
       <c r="E284" s="15"/>
       <c r="F284" s="15"/>
       <c r="G284" s="83"/>
@@ -7755,6 +7755,172 @@
   </sheetData>
   <autoFilter ref="B5:G283"/>
   <mergeCells count="190">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C196:D196"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C138:D138"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="C187:D187"/>
+    <mergeCell ref="C188:D188"/>
+    <mergeCell ref="C189:D189"/>
+    <mergeCell ref="C190:D190"/>
+    <mergeCell ref="C191:D191"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C211:D211"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C183:D183"/>
+    <mergeCell ref="C185:D185"/>
+    <mergeCell ref="C182:D182"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="C136:D136"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="B131:G131"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="C148:D148"/>
+    <mergeCell ref="C268:D268"/>
+    <mergeCell ref="C269:D269"/>
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="C160:D160"/>
+    <mergeCell ref="C161:D161"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C162:D162"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="C254:D254"/>
+    <mergeCell ref="C256:D256"/>
+    <mergeCell ref="C257:D257"/>
+    <mergeCell ref="C263:D263"/>
+    <mergeCell ref="C264:D264"/>
+    <mergeCell ref="C265:D265"/>
+    <mergeCell ref="C266:D266"/>
+    <mergeCell ref="C262:D262"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C283:D283"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C270:D270"/>
+    <mergeCell ref="C274:D274"/>
+    <mergeCell ref="C276:D276"/>
+    <mergeCell ref="C281:D281"/>
+    <mergeCell ref="C282:D282"/>
+    <mergeCell ref="C272:D272"/>
+    <mergeCell ref="C273:D273"/>
+    <mergeCell ref="C278:D278"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C176:D176"/>
+    <mergeCell ref="C198:D198"/>
+    <mergeCell ref="C193:D193"/>
+    <mergeCell ref="C194:D194"/>
+    <mergeCell ref="C232:D232"/>
+    <mergeCell ref="C233:D233"/>
+    <mergeCell ref="C240:D240"/>
+    <mergeCell ref="C241:D241"/>
+    <mergeCell ref="C248:D248"/>
+    <mergeCell ref="C250:D250"/>
+    <mergeCell ref="C252:D252"/>
+    <mergeCell ref="C223:D223"/>
+    <mergeCell ref="C231:D231"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="C177:D177"/>
+    <mergeCell ref="C178:D178"/>
+    <mergeCell ref="C179:D179"/>
+    <mergeCell ref="C180:D180"/>
+    <mergeCell ref="C181:D181"/>
+    <mergeCell ref="C235:D235"/>
+    <mergeCell ref="C225:D225"/>
+    <mergeCell ref="C212:D212"/>
+    <mergeCell ref="C214:D214"/>
+    <mergeCell ref="C216:D216"/>
+    <mergeCell ref="C200:D200"/>
+    <mergeCell ref="C202:D202"/>
+    <mergeCell ref="C204:D204"/>
+    <mergeCell ref="C206:D206"/>
+    <mergeCell ref="C208:D208"/>
+    <mergeCell ref="C210:D210"/>
+    <mergeCell ref="C217:D217"/>
+    <mergeCell ref="C221:D221"/>
+    <mergeCell ref="C222:D222"/>
+    <mergeCell ref="C218:D218"/>
     <mergeCell ref="C261:D261"/>
     <mergeCell ref="C192:D192"/>
     <mergeCell ref="C259:D259"/>
@@ -7779,172 +7945,6 @@
     <mergeCell ref="C229:D229"/>
     <mergeCell ref="C230:D230"/>
     <mergeCell ref="C228:D228"/>
-    <mergeCell ref="C235:D235"/>
-    <mergeCell ref="C225:D225"/>
-    <mergeCell ref="C212:D212"/>
-    <mergeCell ref="C214:D214"/>
-    <mergeCell ref="C216:D216"/>
-    <mergeCell ref="C200:D200"/>
-    <mergeCell ref="C202:D202"/>
-    <mergeCell ref="C204:D204"/>
-    <mergeCell ref="C206:D206"/>
-    <mergeCell ref="C208:D208"/>
-    <mergeCell ref="C210:D210"/>
-    <mergeCell ref="C217:D217"/>
-    <mergeCell ref="C221:D221"/>
-    <mergeCell ref="C222:D222"/>
-    <mergeCell ref="C218:D218"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="C177:D177"/>
-    <mergeCell ref="C178:D178"/>
-    <mergeCell ref="C179:D179"/>
-    <mergeCell ref="C180:D180"/>
-    <mergeCell ref="C181:D181"/>
-    <mergeCell ref="C283:D283"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C270:D270"/>
-    <mergeCell ref="C274:D274"/>
-    <mergeCell ref="C276:D276"/>
-    <mergeCell ref="C281:D281"/>
-    <mergeCell ref="C282:D282"/>
-    <mergeCell ref="C272:D272"/>
-    <mergeCell ref="C273:D273"/>
-    <mergeCell ref="C278:D278"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="C176:D176"/>
-    <mergeCell ref="C198:D198"/>
-    <mergeCell ref="C193:D193"/>
-    <mergeCell ref="C194:D194"/>
-    <mergeCell ref="C232:D232"/>
-    <mergeCell ref="C233:D233"/>
-    <mergeCell ref="C240:D240"/>
-    <mergeCell ref="C241:D241"/>
-    <mergeCell ref="C248:D248"/>
-    <mergeCell ref="C250:D250"/>
-    <mergeCell ref="C252:D252"/>
-    <mergeCell ref="C223:D223"/>
-    <mergeCell ref="C231:D231"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="C148:D148"/>
-    <mergeCell ref="C268:D268"/>
-    <mergeCell ref="C269:D269"/>
-    <mergeCell ref="C151:D151"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="C154:D154"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="C160:D160"/>
-    <mergeCell ref="C161:D161"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C162:D162"/>
-    <mergeCell ref="C164:D164"/>
-    <mergeCell ref="C172:D172"/>
-    <mergeCell ref="C254:D254"/>
-    <mergeCell ref="C256:D256"/>
-    <mergeCell ref="C257:D257"/>
-    <mergeCell ref="C263:D263"/>
-    <mergeCell ref="C264:D264"/>
-    <mergeCell ref="C265:D265"/>
-    <mergeCell ref="C266:D266"/>
-    <mergeCell ref="C262:D262"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="C136:D136"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="B131:G131"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C211:D211"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C183:D183"/>
-    <mergeCell ref="C185:D185"/>
-    <mergeCell ref="C182:D182"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C196:D196"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C138:D138"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C140:D140"/>
-    <mergeCell ref="C187:D187"/>
-    <mergeCell ref="C188:D188"/>
-    <mergeCell ref="C189:D189"/>
-    <mergeCell ref="C190:D190"/>
-    <mergeCell ref="C191:D191"/>
-    <mergeCell ref="C145:D145"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:G19 B6:G11 B20:C20 E20:G20 B21:G62 B64:G130 B132:G270 B272:G284">
     <cfRule type="expression" dxfId="0" priority="444">

</xml_diff>